<commit_message>
Updates to board members
</commit_message>
<xml_diff>
--- a/lib/assets/board-member-terms.xlsx
+++ b/lib/assets/board-member-terms.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elnaz/Documents/dev/policeboard/lib/assets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20660" yWindow="10180" windowWidth="17760" windowHeight="11400" tabRatio="500"/>
+    <workbookView xWindow="20655" yWindow="10185" windowWidth="17760" windowHeight="11400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Last name</t>
   </si>
@@ -87,6 +82,9 @@
   </si>
   <si>
     <t>Sweeney</t>
+  </si>
+  <si>
+    <t>Lightfoot</t>
   </si>
 </sst>
 </file>
@@ -647,26 +645,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="1"/>
-    <col min="5" max="5" width="14.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" style="1"/>
-    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="23.1640625" style="1"/>
+    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" style="1"/>
+    <col min="5" max="5" width="14.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" style="1"/>
+    <col min="7" max="7" width="14.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.125" style="1"/>
+    <col min="9" max="9" width="14.375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="23.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +676,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -697,7 +695,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,7 +714,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -735,7 +733,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -754,7 +752,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -771,7 +769,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -790,7 +788,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -803,7 +801,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -820,7 +818,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -839,7 +837,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -847,12 +845,12 @@
         <v>40730</v>
       </c>
       <c r="C11" s="4">
-        <v>41861</v>
+        <v>42957</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -865,7 +863,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -884,7 +882,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -903,7 +901,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -922,7 +920,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -935,7 +933,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -948,7 +946,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -965,7 +963,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -984,7 +982,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +999,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +1018,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -1039,7 +1037,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1055,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1073,7 +1071,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1082,7 @@
         <v>41131</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1092,12 +1090,12 @@
         <v>41164</v>
       </c>
       <c r="C26" s="4">
-        <v>42957</v>
+        <v>43039</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1110,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1129,7 +1127,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1137,10 +1135,10 @@
         <v>40730</v>
       </c>
       <c r="C29" s="4">
-        <v>41861</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>42308</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1157,7 +1155,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1170,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1189,7 +1187,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1205,6 +1203,17 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="4">
+        <v>42194</v>
+      </c>
+      <c r="C34" s="4">
+        <v>42957</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:J21">

</xml_diff>